<commit_message>
added plotting error checking.  fixed scores plot.
</commit_message>
<xml_diff>
--- a/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2.xlsx
+++ b/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="5" r:id="rId1"/>
     <sheet name="PCA_Results" sheetId="4" r:id="rId2"/>
     <sheet name="Quan Table" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="234">
   <si>
     <t>FileName_CName</t>
   </si>
@@ -785,13 +787,26 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.6031556227391348E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.68695846400288785"/>
+          <c:h val="0.89719889180519097"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Dark Control</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -799,10 +814,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Scores!$C$2:$C$35</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>-5.3814054540843426E-2</c:v>
                 </c:pt>
@@ -821,99 +836,15 @@
                 <c:pt idx="5">
                   <c:v>-4.6522877513156986E-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.33042778478664264</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.64900036495037849</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-2.9215289148648071E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.13187138621122046</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.26468421321357438</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.3153937595776915</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2.4988071544928868E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.15201282336921926</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.1531419514629653</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.11612812829653432</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-0.3413878390047424</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-7.1781402255149725E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.29526701879170519</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-1.3489810820942738E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-3.1569872485578312E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-1.311280292609715E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-4.0273221129393183E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-2.4832651204975318E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-0.10095360369398636</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-7.0354452942760519E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-3.4293843466412259E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-5.1062259292289592E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1.3378780649948049E-4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-1.1517450243989485E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-3.5341797924520686E-4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-7.0647030246422744E-4</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-8.5003575089564708E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-1.0706912931587261E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Scores!$D$2:$D$35</c:f>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>-7.0096676408189201E-2</c:v>
                 </c:pt>
@@ -932,89 +863,188 @@
                 <c:pt idx="5">
                   <c:v>7.2059508289946715E-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fast 2h</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.33042778478664264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.64900036495037849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.9215289148648071E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.13187138621122046</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.26468421321357438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
                   <c:v>0.32630406043721005</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="1">
                   <c:v>0.16179343310339198</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="2">
                   <c:v>6.4984349344951398E-2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="3">
                   <c:v>6.9766710328439785E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="4">
                   <c:v>9.5705152121924056E-2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Fash 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.3153937595776915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.4988071544928868E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.15201282336921926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.1531419514629653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.11612812829653432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$13:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
                   <c:v>-0.67442399878534898</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="1">
                   <c:v>3.9980423971115281E-4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="2">
                   <c:v>-3.0325504427265063E-2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="3">
                   <c:v>5.8009126454769633E-2</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="4">
                   <c:v>-0.22577017823527029</c:v>
                 </c:pt>
-                <c:pt idx="16">
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Fast 8h</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.3413878390047424</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.1781402255149725E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.29526701879170519</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3489810820942738E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.1569872485578312E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
                   <c:v>0.28057742382135314</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="1">
                   <c:v>5.3024492770488547E-2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="2">
                   <c:v>-0.44693011661655052</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="3">
                   <c:v>1.7299704021513311E-2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="4">
                   <c:v>-1.1768338432482076E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6.623997440388771E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-1.4027054749845597E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.0418014977555449E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.2063339428292498</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-7.5011873751382446E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.7167956620518234E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-7.5106962749426501E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1.156429931860911E-5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.6991809346954051E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-2.3030833125824415E-4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7.9424171934953759E-5</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-1.5877172248125692E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-4.1502606008947604E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,11 +1059,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77796480"/>
-        <c:axId val="77794688"/>
+        <c:axId val="140862208"/>
+        <c:axId val="140863744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77796480"/>
+        <c:axId val="140862208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,12 +1073,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77794688"/>
+        <c:crossAx val="140863744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77794688"/>
+        <c:axId val="140863744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1089,214 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77796480"/>
+        <c:crossAx val="140862208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dark Control</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-5.3814054540843426E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.7011312709974754E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.179386370442931E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.821587892282272E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.6626477242977886E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.6522877513156986E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-7.0096676408189201E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2025732076147453E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0268588025531693E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6974610817706375E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.7151929635578871E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2059508289946715E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fast 2 h</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$8:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.33042778478664264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.64900036495037849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.9215289148648071E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.13187138621122046</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.26468421321357438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$8:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.32630406043721005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16179343310339198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4984349344951398E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9766710328439785E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5705152121924056E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="141196288"/>
+        <c:axId val="141210368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="141196288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141210368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="141210368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141196288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,20 +1322,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1405,13 +1677,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -5266,7 +5537,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21833,4 +22103,748 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2">
+        <v>-5.3814054540843426E-2</v>
+      </c>
+      <c r="C2">
+        <v>-7.0096676408189201E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3">
+        <v>-5.7011312709974754E-2</v>
+      </c>
+      <c r="C3">
+        <v>8.2025732076147453E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4">
+        <v>-4.179386370442931E-4</v>
+      </c>
+      <c r="C4">
+        <v>6.0268588025531693E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5">
+        <v>-6.821587892282272E-3</v>
+      </c>
+      <c r="C5">
+        <v>3.6974610817706375E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>-1.6626477242977886E-3</v>
+      </c>
+      <c r="C6">
+        <v>-5.7151929635578871E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7">
+        <v>-4.6522877513156986E-3</v>
+      </c>
+      <c r="C7">
+        <v>7.2059508289946715E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8">
+        <v>-0.33042778478664264</v>
+      </c>
+      <c r="C8">
+        <v>0.32630406043721005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9">
+        <v>-0.64900036495037849</v>
+      </c>
+      <c r="C9">
+        <v>0.16179343310339198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10">
+        <v>-2.9215289148648071E-2</v>
+      </c>
+      <c r="C10">
+        <v>6.4984349344951398E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11">
+        <v>-0.13187138621122046</v>
+      </c>
+      <c r="C11">
+        <v>6.9766710328439785E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12">
+        <v>-0.26468421321357438</v>
+      </c>
+      <c r="C12">
+        <v>9.5705152121924056E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13">
+        <v>-0.3153937595776915</v>
+      </c>
+      <c r="C13">
+        <v>-0.67442399878534898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>-2.4988071544928868E-3</v>
+      </c>
+      <c r="C14">
+        <v>3.9980423971115281E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15">
+        <v>-0.15201282336921926</v>
+      </c>
+      <c r="C15">
+        <v>-3.0325504427265063E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>-0.1531419514629653</v>
+      </c>
+      <c r="C16">
+        <v>5.8009126454769633E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17">
+        <v>-0.11612812829653432</v>
+      </c>
+      <c r="C17">
+        <v>-0.22577017823527029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18">
+        <v>-0.3413878390047424</v>
+      </c>
+      <c r="C18">
+        <v>0.28057742382135314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19">
+        <v>-7.1781402255149725E-3</v>
+      </c>
+      <c r="C19">
+        <v>5.3024492770488547E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20">
+        <v>-0.29526701879170519</v>
+      </c>
+      <c r="C20">
+        <v>-0.44693011661655052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21">
+        <v>-1.3489810820942738E-3</v>
+      </c>
+      <c r="C21">
+        <v>1.7299704021513311E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22">
+        <v>-3.1569872485578312E-2</v>
+      </c>
+      <c r="C22">
+        <v>-1.1768338432482076E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23">
+        <v>-1.311280292609715E-2</v>
+      </c>
+      <c r="C23">
+        <v>6.623997440388771E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24">
+        <v>-4.0273221129393183E-3</v>
+      </c>
+      <c r="C24">
+        <v>-1.4027054749845597E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25">
+        <v>-2.4832651204975318E-3</v>
+      </c>
+      <c r="C25">
+        <v>2.0418014977555449E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26">
+        <v>-0.10095360369398636</v>
+      </c>
+      <c r="C26">
+        <v>0.2063339428292498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27">
+        <v>-7.0354452942760519E-3</v>
+      </c>
+      <c r="C27">
+        <v>-7.5011873751382446E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28">
+        <v>-3.4293843466412259E-3</v>
+      </c>
+      <c r="C28">
+        <v>9.7167956620518234E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29">
+        <v>-5.1062259292289592E-3</v>
+      </c>
+      <c r="C29">
+        <v>-7.5106962749426501E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30">
+        <v>-1.3378780649948049E-4</v>
+      </c>
+      <c r="C30">
+        <v>-1.156429931860911E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31">
+        <v>-1.1517450243989485E-2</v>
+      </c>
+      <c r="C31">
+        <v>2.6991809346954051E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32">
+        <v>-3.5341797924520686E-4</v>
+      </c>
+      <c r="C32">
+        <v>-2.3030833125824415E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33">
+        <v>-7.0647030246422744E-4</v>
+      </c>
+      <c r="C33">
+        <v>7.9424171934953759E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34">
+        <v>-8.5003575089564708E-3</v>
+      </c>
+      <c r="C34">
+        <v>-1.5877172248125692E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35">
+        <v>-1.0706912931587261E-2</v>
+      </c>
+      <c r="C35">
+        <v>-4.1502606008947604E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U17"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2">
+        <v>-5.3814054540843426E-2</v>
+      </c>
+      <c r="D2">
+        <v>-7.0096676408189201E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>160</v>
+      </c>
+      <c r="R2" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" t="s">
+        <v>160</v>
+      </c>
+      <c r="U2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3">
+        <v>-5.7011312709974754E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.2025732076147453E-2</v>
+      </c>
+      <c r="F3">
+        <v>-5.3814054540843426E-2</v>
+      </c>
+      <c r="G3">
+        <v>-5.7011312709974754E-2</v>
+      </c>
+      <c r="H3">
+        <v>-4.179386370442931E-4</v>
+      </c>
+      <c r="I3">
+        <v>-6.821587892282272E-3</v>
+      </c>
+      <c r="J3">
+        <v>-1.6626477242977886E-3</v>
+      </c>
+      <c r="K3">
+        <v>-4.6522877513156986E-3</v>
+      </c>
+      <c r="L3">
+        <v>-0.33042778478664264</v>
+      </c>
+      <c r="M3">
+        <v>-0.64900036495037849</v>
+      </c>
+      <c r="N3">
+        <v>-2.9215289148648071E-2</v>
+      </c>
+      <c r="O3">
+        <v>-0.13187138621122046</v>
+      </c>
+      <c r="P3">
+        <v>-0.26468421321357438</v>
+      </c>
+      <c r="Q3">
+        <v>-0.3153937595776915</v>
+      </c>
+      <c r="R3">
+        <v>-2.4988071544928868E-3</v>
+      </c>
+      <c r="S3">
+        <v>-0.15201282336921926</v>
+      </c>
+      <c r="T3">
+        <v>-0.1531419514629653</v>
+      </c>
+      <c r="U3">
+        <v>-0.11612812829653432</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4">
+        <v>-4.179386370442931E-4</v>
+      </c>
+      <c r="D4">
+        <v>6.0268588025531693E-4</v>
+      </c>
+      <c r="F4">
+        <v>-7.0096676408189201E-2</v>
+      </c>
+      <c r="G4">
+        <v>8.2025732076147453E-2</v>
+      </c>
+      <c r="H4">
+        <v>6.0268588025531693E-4</v>
+      </c>
+      <c r="I4">
+        <v>3.6974610817706375E-3</v>
+      </c>
+      <c r="J4">
+        <v>-5.7151929635578871E-3</v>
+      </c>
+      <c r="K4">
+        <v>7.2059508289946715E-3</v>
+      </c>
+      <c r="L4">
+        <v>0.32630406043721005</v>
+      </c>
+      <c r="M4">
+        <v>0.16179343310339198</v>
+      </c>
+      <c r="N4">
+        <v>6.4984349344951398E-2</v>
+      </c>
+      <c r="O4">
+        <v>6.9766710328439785E-2</v>
+      </c>
+      <c r="P4">
+        <v>9.5705152121924056E-2</v>
+      </c>
+      <c r="Q4">
+        <v>-0.67442399878534898</v>
+      </c>
+      <c r="R4">
+        <v>3.9980423971115281E-4</v>
+      </c>
+      <c r="S4">
+        <v>-3.0325504427265063E-2</v>
+      </c>
+      <c r="T4">
+        <v>5.8009126454769633E-2</v>
+      </c>
+      <c r="U4">
+        <v>-0.22577017823527029</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5">
+        <v>-6.821587892282272E-3</v>
+      </c>
+      <c r="D5">
+        <v>3.6974610817706375E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>-1.6626477242977886E-3</v>
+      </c>
+      <c r="D6">
+        <v>-5.7151929635578871E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7">
+        <v>-4.6522877513156986E-3</v>
+      </c>
+      <c r="D7">
+        <v>7.2059508289946715E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8">
+        <v>-0.33042778478664264</v>
+      </c>
+      <c r="D8">
+        <v>0.32630406043721005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9">
+        <v>-0.64900036495037849</v>
+      </c>
+      <c r="D9">
+        <v>0.16179343310339198</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10">
+        <v>-2.9215289148648071E-2</v>
+      </c>
+      <c r="D10">
+        <v>6.4984349344951398E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11">
+        <v>-0.13187138621122046</v>
+      </c>
+      <c r="D11">
+        <v>6.9766710328439785E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12">
+        <v>-0.26468421321357438</v>
+      </c>
+      <c r="D12">
+        <v>9.5705152121924056E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13">
+        <v>-0.3153937595776915</v>
+      </c>
+      <c r="D13">
+        <v>-0.67442399878534898</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14">
+        <v>-2.4988071544928868E-3</v>
+      </c>
+      <c r="D14">
+        <v>3.9980423971115281E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15">
+        <v>-0.15201282336921926</v>
+      </c>
+      <c r="D15">
+        <v>-3.0325504427265063E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16">
+        <v>-0.1531419514629653</v>
+      </c>
+      <c r="D16">
+        <v>5.8009126454769633E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>-0.11612812829653432</v>
+      </c>
+      <c r="D17">
+        <v>-0.22577017823527029</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
scores plot outputs to a chartsheet instead of a worksheet.
</commit_message>
<xml_diff>
--- a/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2.xlsx
+++ b/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2.xlsx
@@ -10,15 +10,13 @@
     <sheet name="Scores" sheetId="5" r:id="rId1"/>
     <sheet name="PCA_Results" sheetId="4" r:id="rId2"/>
     <sheet name="Quan Table" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="234">
   <si>
     <t>FileName_CName</t>
   </si>
@@ -769,623 +767,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.6031556227391348E-2"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.68695846400288785"/>
-          <c:h val="0.89719889180519097"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Dark Control</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-5.3814054540843426E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-5.7011312709974754E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4.179386370442931E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-6.821587892282272E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.6626477242977886E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-4.6522877513156986E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-7.0096676408189201E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2025732076147453E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0268588025531693E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.6974610817706375E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-5.7151929635578871E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.2059508289946715E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Fast 2h</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$8:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.33042778478664264</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.64900036495037849</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.9215289148648071E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.13187138621122046</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.26468421321357438</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$8:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.32630406043721005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16179343310339198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.4984349344951398E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.9766710328439785E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5705152121924056E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Fash 4</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$13:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.3153937595776915</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.4988071544928868E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.15201282336921926</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.1531419514629653</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.11612812829653432</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$13:$C$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.67442399878534898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9980423971115281E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.0325504427265063E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.8009126454769633E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.22577017823527029</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Fast 8h</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$18:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.3413878390047424</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-7.1781402255149725E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.29526701879170519</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1.3489810820942738E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-3.1569872485578312E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$18:$C$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.28057742382135314</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3024492770488547E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.44693011661655052</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7299704021513311E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.1768338432482076E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="140862208"/>
-        <c:axId val="140863744"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="140862208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140863744"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="140863744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140862208"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Dark Control</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-5.3814054540843426E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-5.7011312709974754E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4.179386370442931E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-6.821587892282272E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.6626477242977886E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-4.6522877513156986E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$D$2:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-7.0096676408189201E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2025732076147453E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0268588025531693E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.6974610817706375E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-5.7151929635578871E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.2059508289946715E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Fast 2 h</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$8:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.33042778478664264</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.64900036495037849</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.9215289148648071E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.13187138621122046</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.26468421321357438</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$D$8:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.32630406043721005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16179343310339198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.4984349344951398E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.9766710328439785E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5705152121924056E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="141196288"/>
-        <c:axId val="141210368"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="141196288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141210368"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="141210368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141196288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22103,748 +21484,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2">
-        <v>-5.3814054540843426E-2</v>
-      </c>
-      <c r="C2">
-        <v>-7.0096676408189201E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3">
-        <v>-5.7011312709974754E-2</v>
-      </c>
-      <c r="C3">
-        <v>8.2025732076147453E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4">
-        <v>-4.179386370442931E-4</v>
-      </c>
-      <c r="C4">
-        <v>6.0268588025531693E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5">
-        <v>-6.821587892282272E-3</v>
-      </c>
-      <c r="C5">
-        <v>3.6974610817706375E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6">
-        <v>-1.6626477242977886E-3</v>
-      </c>
-      <c r="C6">
-        <v>-5.7151929635578871E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7">
-        <v>-4.6522877513156986E-3</v>
-      </c>
-      <c r="C7">
-        <v>7.2059508289946715E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8">
-        <v>-0.33042778478664264</v>
-      </c>
-      <c r="C8">
-        <v>0.32630406043721005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9">
-        <v>-0.64900036495037849</v>
-      </c>
-      <c r="C9">
-        <v>0.16179343310339198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10">
-        <v>-2.9215289148648071E-2</v>
-      </c>
-      <c r="C10">
-        <v>6.4984349344951398E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11">
-        <v>-0.13187138621122046</v>
-      </c>
-      <c r="C11">
-        <v>6.9766710328439785E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12">
-        <v>-0.26468421321357438</v>
-      </c>
-      <c r="C12">
-        <v>9.5705152121924056E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13">
-        <v>-0.3153937595776915</v>
-      </c>
-      <c r="C13">
-        <v>-0.67442399878534898</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14">
-        <v>-2.4988071544928868E-3</v>
-      </c>
-      <c r="C14">
-        <v>3.9980423971115281E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15">
-        <v>-0.15201282336921926</v>
-      </c>
-      <c r="C15">
-        <v>-3.0325504427265063E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B16">
-        <v>-0.1531419514629653</v>
-      </c>
-      <c r="C16">
-        <v>5.8009126454769633E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17">
-        <v>-0.11612812829653432</v>
-      </c>
-      <c r="C17">
-        <v>-0.22577017823527029</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18">
-        <v>-0.3413878390047424</v>
-      </c>
-      <c r="C18">
-        <v>0.28057742382135314</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19">
-        <v>-7.1781402255149725E-3</v>
-      </c>
-      <c r="C19">
-        <v>5.3024492770488547E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B20">
-        <v>-0.29526701879170519</v>
-      </c>
-      <c r="C20">
-        <v>-0.44693011661655052</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B21">
-        <v>-1.3489810820942738E-3</v>
-      </c>
-      <c r="C21">
-        <v>1.7299704021513311E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22">
-        <v>-3.1569872485578312E-2</v>
-      </c>
-      <c r="C22">
-        <v>-1.1768338432482076E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23">
-        <v>-1.311280292609715E-2</v>
-      </c>
-      <c r="C23">
-        <v>6.623997440388771E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B24">
-        <v>-4.0273221129393183E-3</v>
-      </c>
-      <c r="C24">
-        <v>-1.4027054749845597E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25">
-        <v>-2.4832651204975318E-3</v>
-      </c>
-      <c r="C25">
-        <v>2.0418014977555449E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26">
-        <v>-0.10095360369398636</v>
-      </c>
-      <c r="C26">
-        <v>0.2063339428292498</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>164</v>
-      </c>
-      <c r="B27">
-        <v>-7.0354452942760519E-3</v>
-      </c>
-      <c r="C27">
-        <v>-7.5011873751382446E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28">
-        <v>-3.4293843466412259E-3</v>
-      </c>
-      <c r="C28">
-        <v>9.7167956620518234E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>166</v>
-      </c>
-      <c r="B29">
-        <v>-5.1062259292289592E-3</v>
-      </c>
-      <c r="C29">
-        <v>-7.5106962749426501E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>166</v>
-      </c>
-      <c r="B30">
-        <v>-1.3378780649948049E-4</v>
-      </c>
-      <c r="C30">
-        <v>-1.156429931860911E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>168</v>
-      </c>
-      <c r="B31">
-        <v>-1.1517450243989485E-2</v>
-      </c>
-      <c r="C31">
-        <v>2.6991809346954051E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32">
-        <v>-3.5341797924520686E-4</v>
-      </c>
-      <c r="C32">
-        <v>-2.3030833125824415E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>168</v>
-      </c>
-      <c r="B33">
-        <v>-7.0647030246422744E-4</v>
-      </c>
-      <c r="C33">
-        <v>7.9424171934953759E-5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34">
-        <v>-8.5003575089564708E-3</v>
-      </c>
-      <c r="C34">
-        <v>-1.5877172248125692E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35">
-        <v>-1.0706912931587261E-2</v>
-      </c>
-      <c r="C35">
-        <v>-4.1502606008947604E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U17"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2">
-        <v>-5.3814054540843426E-2</v>
-      </c>
-      <c r="D2">
-        <v>-7.0096676408189201E-2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K2" t="s">
-        <v>155</v>
-      </c>
-      <c r="L2" t="s">
-        <v>158</v>
-      </c>
-      <c r="M2" t="s">
-        <v>158</v>
-      </c>
-      <c r="N2" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" t="s">
-        <v>158</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>160</v>
-      </c>
-      <c r="R2" t="s">
-        <v>160</v>
-      </c>
-      <c r="S2" t="s">
-        <v>160</v>
-      </c>
-      <c r="T2" t="s">
-        <v>160</v>
-      </c>
-      <c r="U2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3">
-        <v>-5.7011312709974754E-2</v>
-      </c>
-      <c r="D3">
-        <v>8.2025732076147453E-2</v>
-      </c>
-      <c r="F3">
-        <v>-5.3814054540843426E-2</v>
-      </c>
-      <c r="G3">
-        <v>-5.7011312709974754E-2</v>
-      </c>
-      <c r="H3">
-        <v>-4.179386370442931E-4</v>
-      </c>
-      <c r="I3">
-        <v>-6.821587892282272E-3</v>
-      </c>
-      <c r="J3">
-        <v>-1.6626477242977886E-3</v>
-      </c>
-      <c r="K3">
-        <v>-4.6522877513156986E-3</v>
-      </c>
-      <c r="L3">
-        <v>-0.33042778478664264</v>
-      </c>
-      <c r="M3">
-        <v>-0.64900036495037849</v>
-      </c>
-      <c r="N3">
-        <v>-2.9215289148648071E-2</v>
-      </c>
-      <c r="O3">
-        <v>-0.13187138621122046</v>
-      </c>
-      <c r="P3">
-        <v>-0.26468421321357438</v>
-      </c>
-      <c r="Q3">
-        <v>-0.3153937595776915</v>
-      </c>
-      <c r="R3">
-        <v>-2.4988071544928868E-3</v>
-      </c>
-      <c r="S3">
-        <v>-0.15201282336921926</v>
-      </c>
-      <c r="T3">
-        <v>-0.1531419514629653</v>
-      </c>
-      <c r="U3">
-        <v>-0.11612812829653432</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4">
-        <v>-4.179386370442931E-4</v>
-      </c>
-      <c r="D4">
-        <v>6.0268588025531693E-4</v>
-      </c>
-      <c r="F4">
-        <v>-7.0096676408189201E-2</v>
-      </c>
-      <c r="G4">
-        <v>8.2025732076147453E-2</v>
-      </c>
-      <c r="H4">
-        <v>6.0268588025531693E-4</v>
-      </c>
-      <c r="I4">
-        <v>3.6974610817706375E-3</v>
-      </c>
-      <c r="J4">
-        <v>-5.7151929635578871E-3</v>
-      </c>
-      <c r="K4">
-        <v>7.2059508289946715E-3</v>
-      </c>
-      <c r="L4">
-        <v>0.32630406043721005</v>
-      </c>
-      <c r="M4">
-        <v>0.16179343310339198</v>
-      </c>
-      <c r="N4">
-        <v>6.4984349344951398E-2</v>
-      </c>
-      <c r="O4">
-        <v>6.9766710328439785E-2</v>
-      </c>
-      <c r="P4">
-        <v>9.5705152121924056E-2</v>
-      </c>
-      <c r="Q4">
-        <v>-0.67442399878534898</v>
-      </c>
-      <c r="R4">
-        <v>3.9980423971115281E-4</v>
-      </c>
-      <c r="S4">
-        <v>-3.0325504427265063E-2</v>
-      </c>
-      <c r="T4">
-        <v>5.8009126454769633E-2</v>
-      </c>
-      <c r="U4">
-        <v>-0.22577017823527029</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5">
-        <v>-6.821587892282272E-3</v>
-      </c>
-      <c r="D5">
-        <v>3.6974610817706375E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6">
-        <v>-1.6626477242977886E-3</v>
-      </c>
-      <c r="D6">
-        <v>-5.7151929635578871E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7">
-        <v>-4.6522877513156986E-3</v>
-      </c>
-      <c r="D7">
-        <v>7.2059508289946715E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8">
-        <v>-0.33042778478664264</v>
-      </c>
-      <c r="D8">
-        <v>0.32630406043721005</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9">
-        <v>-0.64900036495037849</v>
-      </c>
-      <c r="D9">
-        <v>0.16179343310339198</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10">
-        <v>-2.9215289148648071E-2</v>
-      </c>
-      <c r="D10">
-        <v>6.4984349344951398E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11">
-        <v>-0.13187138621122046</v>
-      </c>
-      <c r="D11">
-        <v>6.9766710328439785E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12">
-        <v>-0.26468421321357438</v>
-      </c>
-      <c r="D12">
-        <v>9.5705152121924056E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13">
-        <v>-0.3153937595776915</v>
-      </c>
-      <c r="D13">
-        <v>-0.67442399878534898</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14">
-        <v>-2.4988071544928868E-3</v>
-      </c>
-      <c r="D14">
-        <v>3.9980423971115281E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15">
-        <v>-0.15201282336921926</v>
-      </c>
-      <c r="D15">
-        <v>-3.0325504427265063E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16">
-        <v>-0.1531419514629653</v>
-      </c>
-      <c r="D16">
-        <v>5.8009126454769633E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17">
-        <v>-0.11612812829653432</v>
-      </c>
-      <c r="D17">
-        <v>-0.22577017823527029</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>